<commit_message>
listos resultados para analisis
</commit_message>
<xml_diff>
--- a/datos/centros.xlsx
+++ b/datos/centros.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\times\Desktop\Optimización - 1113\ICS1113-G40-Gurobi\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="78" documentId="13_ncr:1_{4845B617-9E6E-452E-92DE-26B66AF62B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{577A4CAE-97E3-4B57-9DF8-8E0D5E2C29B1}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="13_ncr:1_{4845B617-9E6E-452E-92DE-26B66AF62B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBFBC270-E116-4BCC-A7AD-4705371DFA62}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" firstSheet="1" activeTab="1" xr2:uid="{D5AFB4D9-A436-4B9F-8A95-3E6868D31B7A}"/>
   </bookViews>
@@ -749,7 +749,7 @@
   <dimension ref="A1:S12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -806,6 +806,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="1"/>
       <c r="H5" s="12"/>
+      <c r="O5" s="12"/>
     </row>
     <row r="6" spans="1:19" ht="15">
       <c r="A6" s="10"/>

</xml_diff>